<commit_message>
CREATCMR-8362 - DACH coverage story Austria defect fixes.
</commit_message>
<xml_diff>
--- a/RequestCMR/config/MassUpdateTemplateAutoSWISS.xlsx
+++ b/RequestCMR/config/MassUpdateTemplateAutoSWISS.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="489">
   <si>
     <t>CMR. No</t>
   </si>
@@ -1189,10 +1189,10 @@
     <t>21 | 21-Unassigned</t>
   </si>
   <si>
-    <t>32 | 32-OBSOLETE</t>
-  </si>
-  <si>
-    <t>34 | 34-Enterprise</t>
+    <t>32 | 32-Select Dedicated</t>
+  </si>
+  <si>
+    <t>34 | 34-Select</t>
   </si>
   <si>
     <t>60 | 60-Valid Unassigned Account</t>
@@ -1252,6 +1252,9 @@
     <t>5K | 5K-Comp Int Sys Design</t>
   </si>
   <si>
+    <t>36 | 36-Build/Service</t>
+  </si>
+  <si>
     <t>Client Tier</t>
   </si>
   <si>
@@ -1282,6 +1285,12 @@
     <t>Customer Classification Code Values</t>
   </si>
   <si>
+    <t>24 | 24-DIPLOMAT</t>
+  </si>
+  <si>
+    <t>41 | 41-PRODUCT AGENT</t>
+  </si>
+  <si>
     <t>11 | 11-COMMERCIAL CUSTOMER</t>
   </si>
   <si>
@@ -1297,10 +1306,7 @@
     <t>17 | 17-PUBLIC SCHOOL</t>
   </si>
   <si>
-    <t>24 | 24-DIPLOMAT</t>
-  </si>
-  <si>
-    <t>41 | 41-PRODUCT AGENT</t>
+    <t>81 | 81-IBM-Internal</t>
   </si>
   <si>
     <t>43 | 43-SOLUTION PROVIDER</t>
@@ -1313,9 +1319,6 @@
   </si>
   <si>
     <t>71 | 71-IBM-EMPLOYEE</t>
-  </si>
-  <si>
-    <t>81 | 81-IBM-Internal</t>
   </si>
   <si>
     <t>33 | 33-IGF Fin. Subsidiary</t>
@@ -1627,40 +1630,40 @@
         <v>384</v>
       </c>
       <c r="D1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="E1" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="F1" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="G1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="H1" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="I1" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="J1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="K1" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="L1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="M1" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="N1" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="O1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="2">
@@ -1674,40 +1677,40 @@
         <v>385</v>
       </c>
       <c r="D2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E2" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="F2" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="G2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="H2" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="I2" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="J2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="K2" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="L2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="M2" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="N2" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="O2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="3">
@@ -1721,40 +1724,40 @@
         <v>386</v>
       </c>
       <c r="D3" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="E3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="F3" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="G3" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="H3" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="I3" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="J3" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="K3" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="L3" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="M3" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="N3" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="O3" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="4">
@@ -1765,34 +1768,34 @@
         <v>387</v>
       </c>
       <c r="D4" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E4" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="F4" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="G4" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="I4" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="J4" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="K4" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="L4" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="N4" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="O4" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="5">
@@ -1803,31 +1806,31 @@
         <v>388</v>
       </c>
       <c r="E5" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="F5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="G5" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="I5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="J5" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="K5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="L5" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="N5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="O5" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="6">
@@ -1838,19 +1841,19 @@
         <v>389</v>
       </c>
       <c r="E6" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="F6" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="I6" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="K6" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="N6" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="7">
@@ -1861,19 +1864,19 @@
         <v>390</v>
       </c>
       <c r="E7" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="F7" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="I7" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="K7" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="N7" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="8">
@@ -1884,19 +1887,19 @@
         <v>391</v>
       </c>
       <c r="E8" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="F8" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="I8" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="K8" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="N8" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="9">
@@ -1907,19 +1910,19 @@
         <v>392</v>
       </c>
       <c r="E9" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="F9" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="I9" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="K9" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="N9" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="10">
@@ -1930,19 +1933,19 @@
         <v>393</v>
       </c>
       <c r="E10" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="F10" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="I10" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="K10" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="N10" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="11">
@@ -1953,19 +1956,19 @@
         <v>394</v>
       </c>
       <c r="E11" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="F11" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="I11" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="K11" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="N11" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="12">
@@ -1976,19 +1979,19 @@
         <v>395</v>
       </c>
       <c r="E12" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="F12" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="I12" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="K12" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="N12" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="13">
@@ -1999,19 +2002,19 @@
         <v>396</v>
       </c>
       <c r="E13" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="F13" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="I13" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="K13" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="N13" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="14">
@@ -2022,19 +2025,19 @@
         <v>397</v>
       </c>
       <c r="E14" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F14" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="I14" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="K14" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="N14" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="15">
@@ -2045,19 +2048,19 @@
         <v>398</v>
       </c>
       <c r="E15" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F15" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="I15" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="K15" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="N15" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="16">
@@ -2068,16 +2071,16 @@
         <v>399</v>
       </c>
       <c r="F16" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="I16" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="K16" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="N16" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="17">
@@ -2088,16 +2091,16 @@
         <v>400</v>
       </c>
       <c r="F17" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="I17" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="K17" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="N17" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="18">
@@ -2108,16 +2111,16 @@
         <v>401</v>
       </c>
       <c r="F18" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="I18" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="K18" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="N18" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="19">
@@ -2128,16 +2131,16 @@
         <v>402</v>
       </c>
       <c r="F19" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="I19" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="K19" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="N19" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="20">
@@ -2148,16 +2151,16 @@
         <v>403</v>
       </c>
       <c r="F20" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="I20" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="K20" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="N20" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="21">
@@ -2168,16 +2171,16 @@
         <v>404</v>
       </c>
       <c r="F21" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="I21" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="K21" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="N21" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="22">
@@ -2188,16 +2191,16 @@
         <v>405</v>
       </c>
       <c r="F22" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="I22" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="K22" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="N22" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="23">
@@ -2208,16 +2211,16 @@
         <v>406</v>
       </c>
       <c r="F23" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="I23" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="K23" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="N23" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="24">
@@ -2228,16 +2231,16 @@
         <v>407</v>
       </c>
       <c r="F24" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="I24" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="K24" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="N24" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="25">
@@ -2248,16 +2251,16 @@
         <v>408</v>
       </c>
       <c r="F25" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="I25" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="K25" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="N25" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="26">
@@ -2268,16 +2271,16 @@
         <v>409</v>
       </c>
       <c r="F26" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="I26" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="K26" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="N26" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="27">
@@ -2288,21 +2291,24 @@
         <v>410</v>
       </c>
       <c r="F27" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="I27" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="K27" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="N27" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
         <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="29">
@@ -4090,27 +4096,27 @@
         <v>383</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="2002">
       <c r="A2002" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
   </sheetData>
@@ -4134,7 +4140,7 @@
       <formula1>4</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="F2:F2001" allowBlank="true" errorStyle="stop" showErrorMessage="true" errorTitle="Invalid Value" error="Please select values from the list." showInputMessage="true" promptTitle="Note:" prompt="Please select values from the list.">
-      <formula1>Control!$C$2:$C$27</formula1>
+      <formula1>Control!$C$2:$C$28</formula1>
     </dataValidation>
     <dataValidation type="textLength" operator="lessThanOrEqual" sqref="G2:G2001" allowBlank="true" errorStyle="stop" showErrorMessage="true" errorTitle="Invalid Value" error="Maximum length of the value is 1 characters." showInputMessage="true" promptTitle="Note:" prompt="Maximum length of the value is 1 characters.">
       <formula1>1</formula1>
@@ -4194,57 +4200,57 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="2002">
       <c r="A2002" t="s" s="3">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
   </sheetData>
@@ -4342,54 +4348,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="2002">
       <c r="A2002" t="s" s="4">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
   </sheetData>
@@ -4485,57 +4491,57 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="2002">
       <c r="A2002" t="s" s="5">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
   </sheetData>
@@ -4633,54 +4639,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="2002">
       <c r="A2002" t="s" s="6">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>